<commit_message>
enhance the system prompt
</commit_message>
<xml_diff>
--- a/Test Json Result/Book1.xlsx
+++ b/Test Json Result/Book1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AI Model Train\OpenAI API\Model Accuricy Test\Test Json Result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1CB5CC8D-9840-4198-9F14-3B6F81273C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD05A3DA-92D2-4F3A-A103-B4E4B2E60240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{5DCF6B82-2882-43D4-8303-5D51470F368C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{5DCF6B82-2882-43D4-8303-5D51470F368C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="67">
   <si>
     <t xml:space="preserve">Metric </t>
   </si>
@@ -61,14 +62,6 @@
   </si>
   <si>
     <t>Time (s)</t>
-  </si>
-  <si>
-    <t>Phase 1
-(Test Data 890)</t>
-  </si>
-  <si>
-    <t>Phase 2
-(Test Data 950)</t>
   </si>
   <si>
     <t xml:space="preserve">Model </t>
@@ -198,6 +191,65 @@
   <si>
     <t>Inference Output
 (per 1M tokens)</t>
+  </si>
+  <si>
+    <t>Use Avg. 
+70 Token</t>
+  </si>
+  <si>
+    <t>Phase 1
+(Test Data Set 890)</t>
+  </si>
+  <si>
+    <t>Phase 2
+(Test Data Set 950)</t>
+  </si>
+  <si>
+    <t>Phase 3
+(Test Data Set 950)</t>
+  </si>
+  <si>
+    <t>Token Count</t>
+  </si>
+  <si>
+    <t>Use Avg. 
+40 Token</t>
+  </si>
+  <si>
+    <t>171.03s</t>
+  </si>
+  <si>
+    <t>262.27 (10)</t>
+  </si>
+  <si>
+    <t>Phase 4
+(Test Data Set 950)</t>
+  </si>
+  <si>
+    <t>Phase 5
+(Test Data Set 890)</t>
+  </si>
+  <si>
+    <t>Use Avg. 
+150 Token</t>
+  </si>
+  <si>
+    <t>Data Set 1 (890)</t>
+  </si>
+  <si>
+    <t>Data Set 2 (950)</t>
+  </si>
+  <si>
+    <t>Data Set 3 (925)</t>
+  </si>
+  <si>
+    <t>Use Avg. 40 Token</t>
+  </si>
+  <si>
+    <t>Phase 1</t>
+  </si>
+  <si>
+    <t>Combain ALL (2765)</t>
   </si>
 </sst>
 </file>
@@ -245,7 +297,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,6 +313,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF83CCEB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -318,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -326,38 +384,56 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -693,17 +769,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{220715A3-7209-4109-8AEA-ADC016F95071}">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
     <col min="4" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -717,59 +793,62 @@
     <col min="18" max="18" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="7" t="s">
+      <c r="G1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="7" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="2" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
+      <c r="A2" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -786,42 +865,45 @@
       <c r="F2" s="2">
         <v>96.29</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="7" t="s">
+      <c r="G2" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="13"/>
+      <c r="J2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="P2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="Q2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="R2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="R2" s="7" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2">
-        <v>262.27</v>
+      <c r="C3" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="D3" s="2">
         <v>272.02</v>
@@ -832,40 +914,41 @@
       <c r="F3" s="2">
         <v>247.08</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="G3" s="15"/>
+      <c r="I3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="6">
         <v>2</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="6">
         <v>8</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="O3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="P3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="Q3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="R3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="Q3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>9</v>
+      <c r="A4" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
@@ -882,39 +965,40 @@
       <c r="F4" s="2">
         <v>94.42</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="G4" s="15"/>
+      <c r="I4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="6">
         <v>0.4</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="6">
         <v>1.6</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="L4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="O4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="P4" s="9" t="s">
+      <c r="P4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="R4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="Q4" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="R4" s="9" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
@@ -930,108 +1014,219 @@
       <c r="F5" s="2">
         <v>266.13</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="G5" s="15"/>
+      <c r="I5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="6">
         <v>0.1</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="6">
         <v>0.4</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="L5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="9" t="s">
+      <c r="O5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O5" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="P5" s="9" t="s">
+      <c r="P5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="Q5" s="9" t="s">
+    </row>
+    <row r="6" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2">
+        <v>95.16</v>
+      </c>
+      <c r="E6" s="2">
+        <v>80.95</v>
+      </c>
+      <c r="F6" s="2">
+        <v>94</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="R5" s="9" t="s">
+      <c r="Q6" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="I6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="J6" s="9">
-        <v>0.15</v>
-      </c>
-      <c r="K6" s="9">
-        <v>0.6</v>
-      </c>
-      <c r="L6" s="9" t="s">
+      <c r="R6" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2">
+        <v>268.97000000000003</v>
+      </c>
+      <c r="E7" s="2">
+        <v>249.63</v>
+      </c>
+      <c r="F7" s="2">
+        <v>172.46</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="I7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K7" s="6">
+        <v>2.19</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="M6" s="9" t="s">
+      <c r="O7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O6" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="P6" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q6" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="R6" s="9" t="s">
+      <c r="P7" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="I7" s="8" t="s">
+      <c r="Q7" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="9">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="K7" s="9">
-        <v>2.19</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="N7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O7" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="P7" s="9" t="s">
+      <c r="R7" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="Q7" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="R7" s="9" t="s">
-        <v>46</v>
-      </c>
+    </row>
+    <row r="8" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2">
+        <v>94.42</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2">
+        <v>96</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2">
+        <v>178.02</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="15"/>
+    </row>
+    <row r="10" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2">
+        <v>95.84</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2">
+        <v>97.75</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2">
+        <v>126.12</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2">
+        <v>119.55</v>
+      </c>
+      <c r="G11" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="10">
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="G10:G11"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G2:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1040,7 +1235,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,73 +1247,164 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="8">
         <v>25</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="8">
         <v>3</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="8">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="8">
         <v>5</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="8">
         <v>0.8</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="8">
         <v>3.2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>48</v>
+      <c r="B4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="8">
         <v>3</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="8">
         <v>0.3</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="8">
         <v>1.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8080C278-D778-463F-974A-D57AB2BDF2C8}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="17">
+        <v>95.84</v>
+      </c>
+      <c r="C2" s="17">
+        <v>97.75</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="17">
+        <v>94.42</v>
+      </c>
+      <c r="C3" s="19">
+        <v>96</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="17">
+        <v>93.62</v>
+      </c>
+      <c r="C4" s="17">
+        <v>96.97</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="17">
+        <v>94.43</v>
+      </c>
+      <c r="C5" s="17">
+        <v>96.93</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>